<commit_message>
Update lecture materials and add reference files
Added new Excel reference files, updated Book1.xlsx, and revised MCfCL-05-Lecture.md with improved instructions and new images. Included a PDF version of the lecture and supporting figures for clarity in the documentation.
</commit_message>
<xml_diff>
--- a/MCfCL-05-Lecture/Book1.xlsx
+++ b/MCfCL-05-Lecture/Book1.xlsx
@@ -2,18 +2,21 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tetsu\github\2025-SIT-MCfCL\MCfCL-05-Lecture\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0D70A2D3-0821-46F7-8AB9-AC53D61A81DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F000059A-560B-4449-AE06-A03CA8E41F80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3345" yWindow="6615" windowWidth="25695" windowHeight="18675" xr2:uid="{AFFBC682-2C38-4BCC-8BEE-C3896730271D}"/>
+    <workbookView xWindow="8595" yWindow="7035" windowWidth="28950" windowHeight="18675" activeTab="3" xr2:uid="{AFFBC682-2C38-4BCC-8BEE-C3896730271D}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="相対参照" sheetId="1" r:id="rId1"/>
+    <sheet name="絶対参照" sheetId="2" r:id="rId2"/>
+    <sheet name="混合参照" sheetId="3" r:id="rId3"/>
+    <sheet name="F4-key" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,6 +36,72 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+  <si>
+    <t>A1</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>A2</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>A3</t>
+  </si>
+  <si>
+    <t>A4</t>
+  </si>
+  <si>
+    <t>A5</t>
+  </si>
+  <si>
+    <t>B1</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>B2</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>B3</t>
+  </si>
+  <si>
+    <t>B4</t>
+  </si>
+  <si>
+    <t>B5</t>
+  </si>
+  <si>
+    <t>C1</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>C2</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>C3</t>
+  </si>
+  <si>
+    <t>C4</t>
+  </si>
+  <si>
+    <t>C5</t>
+  </si>
+  <si>
+    <t>参照元</t>
+    <rPh sb="0" eb="2">
+      <t>サンショウ</t>
+    </rPh>
+    <rPh sb="2" eb="3">
+      <t>モト</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -414,10 +483,75 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{340485F0-D910-4127-937B-9125F8FACBC3}">
+  <sheetPr codeName="Sheet1"/>
   <dimension ref="B1:E6"/>
   <sheetViews>
-    <sheetView showFormulas="1" tabSelected="1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView showFormulas="1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
+  <sheetData>
+    <row r="1" spans="2:5" x14ac:dyDescent="0.4">
+      <c r="D1">
+        <f>B1</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="2:5" x14ac:dyDescent="0.4">
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <f>A2</f>
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <f>B2</f>
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <f>C2</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="2:5" x14ac:dyDescent="0.4">
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="D3">
+        <f>B3</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.4">
+      <c r="B4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.4">
+      <c r="B5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.4">
+      <c r="B6">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5728D931-C2F9-43FA-B0C4-27379C37E28E}">
+  <sheetPr codeName="Sheet2"/>
+  <dimension ref="B1:E6"/>
+  <sheetViews>
+    <sheetView showFormulas="1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
@@ -473,4 +607,231 @@
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BCEE542D-5DAC-4F52-A5D0-C81A247F905D}">
+  <sheetPr codeName="Sheet3"/>
+  <dimension ref="A1:F10"/>
+  <sheetViews>
+    <sheetView showFormulas="1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" t="str">
+        <f>A$1</f>
+        <v>A1</v>
+      </c>
+      <c r="E1" t="str">
+        <f t="shared" ref="E1:F1" si="0">B$1</f>
+        <v>B1</v>
+      </c>
+      <c r="F1" t="str">
+        <f t="shared" si="0"/>
+        <v>C1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" t="str">
+        <f t="shared" ref="D2:D5" si="1">A$1</f>
+        <v>A1</v>
+      </c>
+      <c r="E2" t="str">
+        <f t="shared" ref="E2:E5" si="2">B$1</f>
+        <v>B1</v>
+      </c>
+      <c r="F2" t="str">
+        <f t="shared" ref="F2:F5" si="3">C$1</f>
+        <v>C1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" t="str">
+        <f t="shared" si="1"/>
+        <v>A1</v>
+      </c>
+      <c r="E3" t="str">
+        <f t="shared" si="2"/>
+        <v>B1</v>
+      </c>
+      <c r="F3" t="str">
+        <f t="shared" si="3"/>
+        <v>C1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" t="str">
+        <f t="shared" si="1"/>
+        <v>A1</v>
+      </c>
+      <c r="E4" t="str">
+        <f t="shared" si="2"/>
+        <v>B1</v>
+      </c>
+      <c r="F4" t="str">
+        <f t="shared" si="3"/>
+        <v>C1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" t="str">
+        <f t="shared" si="1"/>
+        <v>A1</v>
+      </c>
+      <c r="E5" t="str">
+        <f t="shared" si="2"/>
+        <v>B1</v>
+      </c>
+      <c r="F5" t="str">
+        <f t="shared" si="3"/>
+        <v>C1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A6" t="str">
+        <f>$A1</f>
+        <v>A1</v>
+      </c>
+      <c r="B6" t="str">
+        <f t="shared" ref="B6:C6" si="4">$A1</f>
+        <v>A1</v>
+      </c>
+      <c r="C6" t="str">
+        <f t="shared" si="4"/>
+        <v>A1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A7" t="str">
+        <f t="shared" ref="A7:C10" si="5">$A2</f>
+        <v>A2</v>
+      </c>
+      <c r="B7" t="str">
+        <f t="shared" si="5"/>
+        <v>A2</v>
+      </c>
+      <c r="C7" t="str">
+        <f t="shared" si="5"/>
+        <v>A2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A8" t="str">
+        <f t="shared" si="5"/>
+        <v>A3</v>
+      </c>
+      <c r="B8" t="str">
+        <f t="shared" si="5"/>
+        <v>A3</v>
+      </c>
+      <c r="C8" t="str">
+        <f t="shared" si="5"/>
+        <v>A3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A9" t="str">
+        <f t="shared" si="5"/>
+        <v>A4</v>
+      </c>
+      <c r="B9" t="str">
+        <f t="shared" si="5"/>
+        <v>A4</v>
+      </c>
+      <c r="C9" t="str">
+        <f t="shared" si="5"/>
+        <v>A4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A10" t="str">
+        <f t="shared" si="5"/>
+        <v>A5</v>
+      </c>
+      <c r="B10" t="str">
+        <f t="shared" si="5"/>
+        <v>A5</v>
+      </c>
+      <c r="C10" t="str">
+        <f t="shared" si="5"/>
+        <v>A5</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41F3F3D3-7A19-48EA-9BAA-886540731359}">
+  <dimension ref="B2:D2"/>
+  <sheetViews>
+    <sheetView showFormulas="1" tabSelected="1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
+  <sheetData>
+    <row r="2" spans="2:4" x14ac:dyDescent="0.4">
+      <c r="B2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" t="str">
+        <f>B$2</f>
+        <v>参照元</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>